<commit_message>
Update Phase 3-Team Planning.xlsx
</commit_message>
<xml_diff>
--- a/Phase 3/Phase 3-Team Planning.xlsx
+++ b/Phase 3/Phase 3-Team Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uOttawa\CSI\4142\CSI4142_Group15\Phase 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1804EC1C-847C-41D4-9BD5-B24A7F66A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4BB0FD-FA3C-4327-8EBD-9EF0E2806874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC7B5491-6718-42D3-AD60-469765C6A1D2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Deliverable checklist</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Half day</t>
-  </si>
-  <si>
-    <t>One days</t>
   </si>
   <si>
     <t>One day</t>
@@ -231,6 +228,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -240,7 +238,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +555,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:G22"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,16 +577,16 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -598,24 +595,24 @@
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -631,7 +628,7 @@
         <v>45383</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>29</v>
@@ -655,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -676,7 +673,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -697,7 +694,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -856,10 +853,10 @@
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>45384</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="7">
         <v>45385</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -876,10 +873,10 @@
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="7">
         <v>45385</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="7">
         <v>45385</v>
       </c>
       <c r="E21" s="3" t="s">

</xml_diff>